<commit_message>
Fixed a few long names and spacing of output text. Rearranged files.
</commit_message>
<xml_diff>
--- a/Sharp lh5801 Opcode Tables.xlsx
+++ b/Sharp lh5801 Opcode Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb359f9996bef8d1/Vintage_Computers/Sharp_Pocket_Computer/PC-1500/PC-1500_DEV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb359f9996bef8d1/Vintage_Computers/Sharp_Pocket_Computer/PC-1500/PC-1500_DEV/Sharp_PC-1500_Lib_Builder/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="786" documentId="8_{41696516-A3DA-4E96-9B00-86BF1436B725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{181B869E-34AC-4B85-B2D4-AC56AD42788E}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="528" windowWidth="17400" windowHeight="11244" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="576" windowWidth="16692" windowHeight="11088" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alpha Order" sheetId="2" r:id="rId1"/>
@@ -6107,10 +6107,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15317,8 +15313,8 @@
   <dimension ref="A1:J424"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G228" sqref="G228"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>